<commit_message>
Upload newest version of classification dataset
</commit_message>
<xml_diff>
--- a/Compiled Classification Dataset.xlsx
+++ b/Compiled Classification Dataset.xlsx
@@ -2616,7 +2616,7 @@
         <v>3.0</v>
       </c>
       <c r="D5" s="5">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -2631,7 +2631,7 @@
         <v>2.0</v>
       </c>
       <c r="D6" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -5552,6 +5552,12 @@
       <c r="B201" s="6" t="s">
         <v>202</v>
       </c>
+      <c r="C201" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D201" s="5">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="3">
@@ -6655,6 +6661,9 @@
       </c>
       <c r="B275" s="6" t="s">
         <v>276</v>
+      </c>
+      <c r="C275" s="5">
+        <v>2.0</v>
       </c>
       <c r="D275" s="5">
         <v>0.0</v>

</xml_diff>